<commit_message>
added results for convmf
</commit_message>
<xml_diff>
--- a/jupyterlab/notebooks/sommelier-results.xlsx
+++ b/jupyterlab/notebooks/sommelier-results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerrychng/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vannarath.poeu/Documents/Projects/sommelier/jupyterlab/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D45428-BB92-754B-90EE-C86AA32D5943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516BF144-6AEE-DD4E-A9F0-C5D350C33B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35180" yWindow="6760" windowWidth="29240" windowHeight="18500" xr2:uid="{ABE5C703-BF3D-A94A-9570-3A7F8E0B7245}"/>
+    <workbookView xWindow="6000" yWindow="7100" windowWidth="28800" windowHeight="16380" xr2:uid="{ABE5C703-BF3D-A94A-9570-3A7F8E0B7245}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Validation</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Recall@50</t>
+  </si>
+  <si>
+    <t>ConvMF</t>
   </si>
 </sst>
 </file>
@@ -444,7 +447,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,6 +581,43 @@
       <c r="I4">
         <v>3.8199999999999998E-2</v>
       </c>
+      <c r="J4">
+        <f t="shared" ref="J4:J5" si="0">7/((1/C4)+(1/D4)+(1/E4)+(1/F4)+(1/G4)+(1/H4)+(1/I4))</f>
+        <v>2.9134495537827692E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.73399999999999999</v>
+      </c>
+      <c r="D5">
+        <v>0.5615</v>
+      </c>
+      <c r="E5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="F5">
+        <v>8.6E-3</v>
+      </c>
+      <c r="G5">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="H5">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="I5">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>7.2302119509827104E-3</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">

</xml_diff>

<commit_message>
Updated Excel Experiment Tracker for presentation
</commit_message>
<xml_diff>
--- a/jupyterlab/notebooks/sommelier-results.xlsx
+++ b/jupyterlab/notebooks/sommelier-results.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vannarath.poeu/Documents/Projects/sommelier/jupyterlab/notebooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerrychng/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{516BF144-6AEE-DD4E-A9F0-C5D350C33B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BD24B6E-81A7-9F43-8867-B009C21D5278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="7100" windowWidth="28800" windowHeight="16380" xr2:uid="{ABE5C703-BF3D-A94A-9570-3A7F8E0B7245}"/>
+    <workbookView xWindow="17880" yWindow="3100" windowWidth="36780" windowHeight="18580" xr2:uid="{ABE5C703-BF3D-A94A-9570-3A7F8E0B7245}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$5</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -127,14 +130,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -145,6 +199,33 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BA9CD7B-F8CD-0E4B-992D-A404A44C0E3D}" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:J5" xr:uid="{3AC64BA4-D99A-0549-A46C-18286DA3E5E8}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Validation"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{1A7A3DCA-4008-114C-9052-5E2D2530E8C4}" name="Model" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{C97999EC-BF1E-4843-B38D-EF3D1544ABC1}" name="Data" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{E151FE2F-2CBB-DF49-AAA9-41C33A75FFDD}" name="RMSE" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{04D1EEAC-9D26-7E47-8785-9396CFF4B4E1}" name="AUC" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{46542D53-39B2-0C4F-8EFC-D2CF76EBC0BF}" name="F1@20" dataDxfId="7"/>
+    <tableColumn id="6" xr3:uid="{492269FE-F389-4C4C-8B7D-671AAF566F93}" name="MRR" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{51EE8669-F234-8544-A027-AE758C05801F}" name="NCRR@20" dataDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{75849CBE-21A3-8D48-80DC-A8B71EBE0B0A}" name="NDCG@20" dataDxfId="4"/>
+    <tableColumn id="9" xr3:uid="{BD39C1A6-C215-D440-ACBB-AB3DF5A66761}" name="Recall@20" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{6054F6C8-3854-5F4E-93F7-830137B1B8A9}" name="Harmonic mean" dataDxfId="2">
+      <calculatedColumnFormula>7/((1/C2)+(1/D2)+(1/E2)+(1/F2)+(1/G2)+(1/H2)+(1/I2))</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -447,105 +528,107 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection sqref="A1:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="12.83203125" customWidth="1"/>
+    <col min="3" max="9" width="12.83203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>2.4152</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.82979999999999998</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>1.0200000000000001E-2</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>3.3700000000000001E-2</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <f>7/((1/C2)+(1/D2)+(1/E2)+(1/F2)+(1/G2)+(1/H2)+(1/I2))</f>
         <v>1.8346866315792767E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2.4077000000000002</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>0.83720000000000006</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>6.7999999999999996E-3</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>2.06E-2</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>9.1000000000000004E-3</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="1">
         <v>1.4800000000000001E-2</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="1">
         <v>3.1300000000000001E-2</v>
       </c>
       <c r="J3">
@@ -554,67 +637,67 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4">
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
         <v>2.8386999999999998</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.69420000000000004</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>1.24E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>4.02E-2</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>1.6199999999999999E-2</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>2.2200000000000001E-2</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <f t="shared" ref="J4:J5" si="0">7/((1/C4)+(1/D4)+(1/E4)+(1/F4)+(1/G4)+(1/H4)+(1/I4))</f>
         <v>2.9134495537827692E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>0.73399999999999999</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.5615</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>8.6E-3</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="2">
         <f t="shared" si="0"/>
         <v>7.2302119509827104E-3</v>
       </c>
@@ -626,25 +709,25 @@
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>17</v>
       </c>
     </row>
@@ -655,29 +738,128 @@
       <c r="B13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>2.8386999999999998</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>0.69420000000000004</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>1.0699999999999999E-2</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="1">
         <v>4.02E-2</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="1">
         <v>3.15E-2</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="1">
         <v>6.83E-2</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C2:C5">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D5">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F5">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G5">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I5">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J5">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Excel Experiment Tracker with CTR results
</commit_message>
<xml_diff>
--- a/jupyterlab/notebooks/sommelier-results.xlsx
+++ b/jupyterlab/notebooks/sommelier-results.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerrychng/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9BD24B6E-81A7-9F43-8867-B009C21D5278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E5E5E1-DA96-F943-A2EC-4C2B26913EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17880" yWindow="3100" windowWidth="36780" windowHeight="18580" xr2:uid="{ABE5C703-BF3D-A94A-9570-3A7F8E0B7245}"/>
+    <workbookView xWindow="2360" yWindow="5220" windowWidth="36780" windowHeight="18580" xr2:uid="{ABE5C703-BF3D-A94A-9570-3A7F8E0B7245}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,9 +43,6 @@
     <t>Validation</t>
   </si>
   <si>
-    <t>RMSE</t>
-  </si>
-  <si>
     <t>AUC</t>
   </si>
   <si>
@@ -95,6 +92,9 @@
   </si>
   <si>
     <t>ConvMF</t>
+  </si>
+  <si>
+    <t>CTR</t>
   </si>
 </sst>
 </file>
@@ -145,7 +145,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -153,39 +183,6 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -202,26 +199,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BA9CD7B-F8CD-0E4B-992D-A404A44C0E3D}" name="Table1" displayName="Table1" ref="A1:J5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:J5" xr:uid="{3AC64BA4-D99A-0549-A46C-18286DA3E5E8}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6BA9CD7B-F8CD-0E4B-992D-A404A44C0E3D}" name="Table1" displayName="Table1" ref="A1:I6" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:I6" xr:uid="{3AC64BA4-D99A-0549-A46C-18286DA3E5E8}">
     <filterColumn colId="1">
       <filters>
         <filter val="Validation"/>
       </filters>
     </filterColumn>
   </autoFilter>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{1A7A3DCA-4008-114C-9052-5E2D2530E8C4}" name="Model" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C97999EC-BF1E-4843-B38D-EF3D1544ABC1}" name="Data" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{E151FE2F-2CBB-DF49-AAA9-41C33A75FFDD}" name="RMSE" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{04D1EEAC-9D26-7E47-8785-9396CFF4B4E1}" name="AUC" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{46542D53-39B2-0C4F-8EFC-D2CF76EBC0BF}" name="F1@20" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{492269FE-F389-4C4C-8B7D-671AAF566F93}" name="MRR" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{51EE8669-F234-8544-A027-AE758C05801F}" name="NCRR@20" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{75849CBE-21A3-8D48-80DC-A8B71EBE0B0A}" name="NDCG@20" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{BD39C1A6-C215-D440-ACBB-AB3DF5A66761}" name="Recall@20" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{6054F6C8-3854-5F4E-93F7-830137B1B8A9}" name="Harmonic mean" dataDxfId="2">
-      <calculatedColumnFormula>7/((1/C2)+(1/D2)+(1/E2)+(1/F2)+(1/G2)+(1/H2)+(1/I2))</calculatedColumnFormula>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I6">
+    <sortCondition descending="1" ref="D1:D6"/>
+  </sortState>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{1A7A3DCA-4008-114C-9052-5E2D2530E8C4}" name="Model" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C97999EC-BF1E-4843-B38D-EF3D1544ABC1}" name="Data" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{04D1EEAC-9D26-7E47-8785-9396CFF4B4E1}" name="AUC" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{46542D53-39B2-0C4F-8EFC-D2CF76EBC0BF}" name="F1@20" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{492269FE-F389-4C4C-8B7D-671AAF566F93}" name="MRR" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{51EE8669-F234-8544-A027-AE758C05801F}" name="NCRR@20" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{75849CBE-21A3-8D48-80DC-A8B71EBE0B0A}" name="NDCG@20" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{BD39C1A6-C215-D440-ACBB-AB3DF5A66761}" name="Recall@20" dataDxfId="1"/>
+    <tableColumn id="10" xr3:uid="{6054F6C8-3854-5F4E-93F7-830137B1B8A9}" name="Harmonic mean" dataDxfId="0">
+      <calculatedColumnFormula>7/((1/#REF!)+(1/C2)+(1/D2)+(1/E2)+(1/F2)+(1/G2)+(1/H2))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -525,36 +524,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AC64BA4-D99A-0549-A46C-18286DA3E5E8}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J5"/>
+      <selection sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="9" width="12.83203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
@@ -563,163 +562,178 @@
       <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>12</v>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>2.4152</v>
+        <v>0.69369999999999998</v>
       </c>
       <c r="D2" s="2">
-        <v>0.82979999999999998</v>
+        <v>1.4E-2</v>
       </c>
       <c r="E2" s="2">
-        <v>7.0000000000000001E-3</v>
+        <v>0.46</v>
       </c>
       <c r="F2" s="2">
-        <v>2.1000000000000001E-2</v>
+        <v>2.0899999999999998E-2</v>
       </c>
       <c r="G2" s="2">
-        <v>1.0200000000000001E-2</v>
+        <v>2.7799999999999998E-2</v>
       </c>
       <c r="H2" s="2">
-        <v>1.6199999999999999E-2</v>
+        <v>4.5600000000000002E-2</v>
       </c>
       <c r="I2" s="2">
-        <v>3.3700000000000001E-2</v>
-      </c>
-      <c r="J2" s="2">
-        <f>7/((1/C2)+(1/D2)+(1/E2)+(1/F2)+(1/G2)+(1/H2)+(1/I2))</f>
-        <v>1.8346866315792767E-2</v>
+        <f>6/((1/C2)+(1/D2)+(1/E2)+(1/F2)+(1/G2)+(1/H2))</f>
+        <v>3.3187315167551308E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>2.4077000000000002</v>
+        <v>0.83720000000000006</v>
       </c>
       <c r="D3" s="1">
-        <v>0.83720000000000006</v>
+        <v>6.7999999999999996E-3</v>
       </c>
       <c r="E3" s="1">
-        <v>6.7999999999999996E-3</v>
+        <v>2.06E-2</v>
       </c>
       <c r="F3" s="1">
-        <v>2.06E-2</v>
+        <v>9.1000000000000004E-3</v>
       </c>
       <c r="G3" s="1">
-        <v>9.1000000000000004E-3</v>
+        <v>1.4800000000000001E-2</v>
       </c>
       <c r="H3" s="1">
-        <v>1.4800000000000001E-2</v>
-      </c>
-      <c r="I3" s="1">
         <v>3.1300000000000001E-2</v>
       </c>
-      <c r="J3">
-        <f>7/((1/C3)+(1/D3)+(1/E3)+(1/F3)+(1/G3)+(1/H3)+(1/I3))</f>
-        <v>1.721513835343318E-2</v>
+      <c r="I3" t="e">
+        <f>7/((1/#REF!)+(1/C3)+(1/D3)+(1/E3)+(1/F3)+(1/G3)+(1/H3))</f>
+        <v>#REF!</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="2">
-        <v>2.8386999999999998</v>
+        <v>0.69420000000000004</v>
       </c>
       <c r="D4" s="2">
-        <v>0.69420000000000004</v>
+        <v>1.24E-2</v>
       </c>
       <c r="E4" s="2">
-        <v>1.24E-2</v>
+        <v>4.02E-2</v>
       </c>
       <c r="F4" s="2">
-        <v>4.02E-2</v>
+        <v>1.6199999999999999E-2</v>
       </c>
       <c r="G4" s="2">
-        <v>1.6199999999999999E-2</v>
+        <v>2.2200000000000001E-2</v>
       </c>
       <c r="H4" s="2">
-        <v>2.2200000000000001E-2</v>
+        <v>3.8199999999999998E-2</v>
       </c>
       <c r="I4" s="2">
-        <v>3.8199999999999998E-2</v>
-      </c>
-      <c r="J4" s="2">
-        <f t="shared" ref="J4:J5" si="0">7/((1/C4)+(1/D4)+(1/E4)+(1/F4)+(1/G4)+(1/H4)+(1/I4))</f>
-        <v>2.9134495537827692E-2</v>
+        <f>6/((1/C4)+(1/D4)+(1/E4)+(1/F4)+(1/G4)+(1/H4))</f>
+        <v>2.5009092804155655E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>0.73399999999999999</v>
+        <v>0.82979999999999998</v>
       </c>
       <c r="D5" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E5" s="2">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1.0200000000000001E-2</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="I5" s="2">
+        <f>6/((1/C5)+(1/D5)+(1/E5)+(1/F5)+(1/G5)+(1/H5))</f>
+        <v>1.5742969722491378E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
         <v>0.5615</v>
       </c>
-      <c r="E5" s="2">
+      <c r="D6" s="2">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="F5" s="2">
+      <c r="E6" s="2">
         <v>8.6E-3</v>
       </c>
-      <c r="G5" s="2">
+      <c r="F6" s="2">
         <v>3.5999999999999999E-3</v>
       </c>
-      <c r="H5" s="2">
+      <c r="G6" s="2">
         <v>6.1999999999999998E-3</v>
       </c>
-      <c r="I5" s="2">
+      <c r="H6" s="2">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="J5" s="2">
-        <f t="shared" si="0"/>
-        <v>7.2302119509827104E-3</v>
+      <c r="I6" s="2">
+        <f>6/((1/C6)+(1/D6)+(1/E6)+(1/F6)+(1/G6)+(1/H6))</f>
+        <v>6.2060577159973821E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>15</v>
@@ -727,53 +741,35 @@
       <c r="H11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>17</v>
-      </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
-        <v>2.8386999999999998</v>
+        <v>0.69420000000000004</v>
       </c>
       <c r="D13" s="1">
-        <v>0.69420000000000004</v>
+        <v>1.0699999999999999E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>1.0699999999999999E-2</v>
+        <v>4.02E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>4.02E-2</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="G13" s="1">
-        <v>1.7999999999999999E-2</v>
+        <v>3.15E-2</v>
       </c>
       <c r="H13" s="1">
-        <v>3.15E-2</v>
-      </c>
-      <c r="I13" s="1">
         <v>6.83E-2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C5">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D5">
+  <conditionalFormatting sqref="C2:C6">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -785,7 +781,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E5">
+  <conditionalFormatting sqref="D2:D6">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -797,7 +793,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F5">
+  <conditionalFormatting sqref="E2:E6">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -809,7 +805,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G5">
+  <conditionalFormatting sqref="F2:F6">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -821,7 +817,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H5">
+  <conditionalFormatting sqref="G2:G6">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -833,7 +829,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I5">
+  <conditionalFormatting sqref="H2:H6">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -845,7 +841,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
+  <conditionalFormatting sqref="I2:I6">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>